<commit_message>
Add 'scoss' field to the data collection template
</commit_message>
<xml_diff>
--- a/2025--TSOSI-data-schema-infra-template.xlsx
+++ b/2025--TSOSI-data-schema-infra-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t xml:space="preserve">institution/name</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">date_received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoss</t>
   </si>
   <si>
     <t xml:space="preserve">contract/id</t>
@@ -172,7 +175,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -210,12 +213,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -303,11 +300,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,12 +431,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -458,10 +455,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="20.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="2" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="19.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="17.59"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="21.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -525,45 +522,49 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>3000</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="6" t="b">
+        <v>30</v>
+      </c>
+      <c r="M2" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="N2" s="7" t="n">
@@ -575,198 +576,229 @@
       <c r="P2" s="8" t="n">
         <v>45108</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="9" t="n">
+      <c r="S2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="8" t="n">
         <v>44927</v>
       </c>
-      <c r="T2" s="8" t="n">
+      <c r="U2" s="8" t="n">
         <v>46022</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>5000</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="6" t="b">
+        <v>30</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>2021</v>
+      </c>
+      <c r="Q3" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>3300</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="6" t="b">
+        <v>30</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P4" s="1" t="n">
         <v>2021</v>
+      </c>
+      <c r="Q4" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>2000</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="6" t="b">
+        <v>30</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P5" s="8" t="n">
         <v>45717</v>
       </c>
-      <c r="Q5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="7"/>
-      <c r="S5" s="1" t="s">
+      <c r="Q5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="10" t="s">
         <v>37</v>
       </c>
+      <c r="S5" s="7"/>
       <c r="T5" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>3100</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="6" t="b">
+        <v>30</v>
+      </c>
+      <c r="M6" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="Q6" s="9" t="b">
+        <v>0</v>
+      </c>
       <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" s="6" t="b">
+        <v>46</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="Q7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="S7" s="8" t="n">
+      <c r="Q7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="T7" s="8" t="n">
         <v>44197</v>
       </c>
-      <c r="T7" s="8" t="n">
+      <c r="U7" s="8" t="n">
         <v>45291</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="6" t="b">
+        <v>46</v>
+      </c>
+      <c r="M8" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P8" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="Q8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="8" t="n">
+      <c r="Q8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="T8" s="8" t="n">
         <v>44197</v>
       </c>
-      <c r="T8" s="8" t="n">
+      <c r="U8" s="8" t="n">
         <v>45291</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" s="6" t="b">
+        <v>46</v>
+      </c>
+      <c r="M9" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="Q9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="8" t="n">
+      <c r="Q9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="T9" s="8" t="n">
         <v>44197</v>
       </c>
-      <c r="T9" s="8" t="n">
+      <c r="U9" s="8" t="n">
         <v>45291</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update table w english boolean values
</commit_message>
<xml_diff>
--- a/2025--TSOSI-data-schema-infra-template.xlsx
+++ b/2025--TSOSI-data-schema-infra-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t xml:space="preserve">institution/name</t>
   </si>
@@ -115,6 +115,9 @@
     <t xml:space="preserve">EUR</t>
   </si>
   <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">L2167</t>
   </si>
   <si>
@@ -161,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">L210</t>
@@ -172,7 +178,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="6">
@@ -263,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,7 +294,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,10 +303,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,13 +435,13 @@
   </sheetPr>
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="Q13" activeCellId="0" sqref="Q13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.15"/>
@@ -563,9 +565,8 @@
       <c r="L2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="M2" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="N2" s="7" t="n">
         <v>45048</v>
@@ -576,14 +577,14 @@
       <c r="P2" s="8" t="n">
         <v>45108</v>
       </c>
-      <c r="Q2" s="9" t="b">
-        <v>0</v>
+      <c r="Q2" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T2" s="8" t="n">
         <v>44927</v>
@@ -605,23 +606,22 @@
       <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="Q3" s="9" t="b">
-        <v>0</v>
+      <c r="Q3" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>3300</v>
@@ -629,23 +629,22 @@
       <c r="L4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="M4" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P4" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="Q4" s="9" t="b">
-        <v>0</v>
+      <c r="Q4" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>2000</v>
@@ -653,36 +652,35 @@
       <c r="L5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="M5" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P5" s="8" t="n">
         <v>45717</v>
       </c>
-      <c r="Q5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>37</v>
+      <c r="Q5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>3100</v>
@@ -690,44 +688,42 @@
       <c r="L6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="M6" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" s="9" t="b">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="Q7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>47</v>
+      <c r="Q7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="T7" s="8" t="n">
         <v>44197</v>
@@ -738,29 +734,28 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M8" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P8" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="Q8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>47</v>
+      <c r="Q8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="T8" s="8" t="n">
         <v>44197</v>
@@ -771,29 +766,28 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="Q9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>47</v>
+      <c r="Q9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="T9" s="8" t="n">
         <v>44197</v>
@@ -807,8 +801,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>